<commit_message>
Updated Project Plan's flowchart.
</commit_message>
<xml_diff>
--- a/project_files/Project Plan Flowchart.xlsx
+++ b/project_files/Project Plan Flowchart.xlsx
@@ -1526,6 +1526,13 @@
     <dgm:pt modelId="{B3567011-4FCA-4059-B7AF-90881D97BF85}" type="pres">
       <dgm:prSet presAssocID="{2068AF2F-21BC-4ACF-AA6A-4F15AF98E83D}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="5"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-SG"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AF1095EC-A7D8-43FD-BF1C-676D4F8A3843}" type="pres">
       <dgm:prSet presAssocID="{BA4F28C5-F2DE-4883-B7D7-E7CA28803ECA}" presName="hierRoot2" presStyleCnt="0">
@@ -5723,6 +5730,56 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Elbow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="5924550" y="3362325"/>
+          <a:ext cx="895350" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1063"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 

</xml_diff>